<commit_message>
prueba de cambio selene
</commit_message>
<xml_diff>
--- a/Organización/Ventas/PTL_Estimación_nombreproyecto.xlsx
+++ b/Organización/Ventas/PTL_Estimación_nombreproyecto.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp EliteBook\Documents\Repositorio\SOSQTP\Organización\Ventas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="898" activeTab="1"/>
   </bookViews>
@@ -22,7 +27,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Instrucciones de plantilla'!$B$5:$J$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Resumen!$B$2:$M$13</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -32,7 +37,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="E66" authorId="0">
+    <comment ref="E66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E74" authorId="0">
+    <comment ref="E74" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E82" authorId="0">
+    <comment ref="E82" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E90" authorId="0">
+    <comment ref="E90" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="378">
   <si>
     <t>Hoja de instrucciones, eliminar antes de finalizar la estimación</t>
   </si>
@@ -1385,6 +1390,9 @@
   </si>
   <si>
     <t>Resolver solicitud, validar con cliente y cerrar tarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2949,6 +2957,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="25" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="50" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="26" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="26" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="26" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="26" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2982,18 +3017,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="22" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3003,17 +3026,23 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="22" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="20" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="169" fontId="34" fillId="17" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -3024,44 +3053,23 @@
     <xf numFmtId="0" fontId="35" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="26" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="19" fillId="26" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="26" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="26" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3143,6 +3151,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3844,7 +3855,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3879,7 +3890,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4135,20 +4146,20 @@
     </row>
     <row r="2" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="183" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="183"/>
+      <c r="M2" s="183"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4212,17 +4223,17 @@
     </row>
     <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="171" t="s">
+      <c r="B5" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="171"/>
-      <c r="F5" s="171"/>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="171"/>
-      <c r="J5" s="171"/>
+      <c r="C5" s="184"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="184"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -4239,15 +4250,15 @@
     </row>
     <row r="6" spans="1:23" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="171"/>
-      <c r="G6" s="171"/>
-      <c r="H6" s="171"/>
-      <c r="I6" s="171"/>
-      <c r="J6" s="171"/>
+      <c r="B6" s="184"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="184"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="184"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="184"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -4264,15 +4275,15 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="171"/>
-      <c r="H7" s="171"/>
-      <c r="I7" s="171"/>
-      <c r="J7" s="171"/>
+      <c r="B7" s="184"/>
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="184"/>
+      <c r="H7" s="184"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="184"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -4289,15 +4300,15 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="171"/>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="171"/>
+      <c r="B8" s="184"/>
+      <c r="C8" s="184"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="184"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -4314,15 +4325,15 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="171"/>
-      <c r="J9" s="171"/>
+      <c r="B9" s="184"/>
+      <c r="C9" s="184"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="184"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -4339,15 +4350,15 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="171"/>
-      <c r="C10" s="171"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="171"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -4367,13 +4378,13 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="172" t="s">
+      <c r="E11" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="172"/>
-      <c r="G11" s="172"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
+      <c r="F11" s="185"/>
+      <c r="G11" s="185"/>
+      <c r="H11" s="185"/>
+      <c r="I11" s="185"/>
       <c r="J11" s="5"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -4394,11 +4405,11 @@
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="172"/>
-      <c r="F12" s="172"/>
-      <c r="G12" s="172"/>
-      <c r="H12" s="172"/>
-      <c r="I12" s="172"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="185"/>
+      <c r="H12" s="185"/>
+      <c r="I12" s="185"/>
       <c r="J12" s="5"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -4419,11 +4430,11 @@
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="172"/>
-      <c r="G13" s="172"/>
-      <c r="H13" s="172"/>
-      <c r="I13" s="172"/>
+      <c r="E13" s="185"/>
+      <c r="F13" s="185"/>
+      <c r="G13" s="185"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="185"/>
       <c r="J13" s="5"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -4444,11 +4455,11 @@
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="172"/>
-      <c r="F14" s="172"/>
-      <c r="G14" s="172"/>
-      <c r="H14" s="172"/>
-      <c r="I14" s="172"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185"/>
+      <c r="H14" s="185"/>
+      <c r="I14" s="185"/>
       <c r="J14" s="8"/>
       <c r="K14" s="9"/>
       <c r="L14" s="1"/>
@@ -4469,11 +4480,11 @@
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
-      <c r="H15" s="172"/>
-      <c r="I15" s="172"/>
+      <c r="E15" s="185"/>
+      <c r="F15" s="185"/>
+      <c r="G15" s="185"/>
+      <c r="H15" s="185"/>
+      <c r="I15" s="185"/>
       <c r="J15" s="8"/>
       <c r="K15" s="9"/>
       <c r="L15" s="1"/>
@@ -4494,11 +4505,11 @@
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="172"/>
-      <c r="G16" s="172"/>
-      <c r="H16" s="172"/>
-      <c r="I16" s="172"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="185"/>
+      <c r="G16" s="185"/>
+      <c r="H16" s="185"/>
+      <c r="I16" s="185"/>
       <c r="J16" s="8"/>
       <c r="K16" s="9"/>
       <c r="L16" s="1"/>
@@ -4519,11 +4530,11 @@
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="172"/>
-      <c r="F17" s="172"/>
-      <c r="G17" s="172"/>
-      <c r="H17" s="172"/>
-      <c r="I17" s="172"/>
+      <c r="E17" s="185"/>
+      <c r="F17" s="185"/>
+      <c r="G17" s="185"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
       <c r="J17" s="8"/>
       <c r="K17" s="9"/>
       <c r="L17" s="1"/>
@@ -4544,11 +4555,11 @@
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
+      <c r="E18" s="185"/>
+      <c r="F18" s="185"/>
+      <c r="G18" s="185"/>
+      <c r="H18" s="185"/>
+      <c r="I18" s="185"/>
       <c r="J18" s="8"/>
       <c r="K18" s="9"/>
       <c r="L18" s="1"/>
@@ -5520,7 +5531,7 @@
   <dimension ref="A1:AD70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5566,22 +5577,22 @@
     </row>
     <row r="2" spans="1:29" s="22" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="188" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="176" t="s">
+      <c r="I2" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
-      <c r="M2" s="176"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="189"/>
+      <c r="L2" s="189"/>
+      <c r="M2" s="189"/>
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
@@ -5601,20 +5612,20 @@
     </row>
     <row r="3" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
+      <c r="B3" s="188"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="177" t="s">
+      <c r="I3" s="190" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="177"/>
-      <c r="K3" s="177"/>
-      <c r="L3" s="177"/>
-      <c r="M3" s="177"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
+      <c r="L3" s="190"/>
+      <c r="M3" s="190"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -5668,11 +5679,11 @@
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
-      <c r="E5" s="173" t="s">
+      <c r="E5" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="173"/>
-      <c r="G5" s="173"/>
+      <c r="F5" s="186"/>
+      <c r="G5" s="186"/>
       <c r="H5" s="35">
         <f>SUM('Costo Etapas proyecto'!B1)</f>
         <v>0</v>
@@ -5802,11 +5813,11 @@
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="173" t="s">
+      <c r="E9" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="173"/>
-      <c r="G9" s="173"/>
+      <c r="F9" s="186"/>
+      <c r="G9" s="186"/>
       <c r="H9" s="35">
         <f>SUM('Gastos operación'!E1)</f>
         <v>0</v>
@@ -5869,11 +5880,11 @@
       <c r="B11" s="29"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
-      <c r="E11" s="174" t="s">
+      <c r="E11" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="174"/>
-      <c r="G11" s="174"/>
+      <c r="F11" s="187"/>
+      <c r="G11" s="187"/>
       <c r="H11" s="31">
         <f>SUM(H10:H10)</f>
         <v>0</v>
@@ -5905,9 +5916,9 @@
       <c r="B12" s="29"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
-      <c r="E12" s="174"/>
-      <c r="F12" s="174"/>
-      <c r="G12" s="174"/>
+      <c r="E12" s="187"/>
+      <c r="F12" s="187"/>
+      <c r="G12" s="187"/>
       <c r="H12" s="34"/>
       <c r="I12" s="30"/>
       <c r="J12" s="30"/>
@@ -6060,7 +6071,9 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -7841,11 +7854,11 @@
       <c r="A4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="210"/>
-      <c r="C4" s="202"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="203"/>
-      <c r="F4" s="204"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="175"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -7993,11 +8006,11 @@
       <c r="A9" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="210"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="207"/>
-      <c r="E9" s="203"/>
-      <c r="F9" s="204"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="174"/>
+      <c r="F9" s="175"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -8241,11 +8254,11 @@
       <c r="A17" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="201"/>
-      <c r="C17" s="202"/>
-      <c r="D17" s="207"/>
-      <c r="E17" s="203"/>
-      <c r="F17" s="204"/>
+      <c r="B17" s="172"/>
+      <c r="C17" s="173"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="174"/>
+      <c r="F17" s="175"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -8390,14 +8403,14 @@
       <c r="A22" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="201"/>
-      <c r="C22" s="202"/>
-      <c r="D22" s="207">
+      <c r="B22" s="172"/>
+      <c r="C22" s="173"/>
+      <c r="D22" s="178">
         <f>Compras!E17</f>
         <v>0</v>
       </c>
-      <c r="E22" s="203"/>
-      <c r="F22" s="204"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="175"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -8417,11 +8430,11 @@
       <c r="A23" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="201"/>
-      <c r="C23" s="202"/>
-      <c r="D23" s="201"/>
-      <c r="E23" s="203"/>
-      <c r="F23" s="204"/>
+      <c r="B23" s="172"/>
+      <c r="C23" s="173"/>
+      <c r="D23" s="172"/>
+      <c r="E23" s="174"/>
+      <c r="F23" s="175"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -8438,7 +8451,7 @@
       <c r="T23" s="1"/>
     </row>
     <row r="24" spans="1:22" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="199" t="s">
+      <c r="A24" s="170" t="s">
         <v>371</v>
       </c>
       <c r="B24" s="151">
@@ -8470,7 +8483,7 @@
       <c r="T24" s="1"/>
     </row>
     <row r="25" spans="1:22" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="200" t="s">
+      <c r="A25" s="171" t="s">
         <v>372</v>
       </c>
       <c r="B25" s="153">
@@ -8505,11 +8518,11 @@
       <c r="A26" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="201"/>
-      <c r="C26" s="202"/>
-      <c r="D26" s="201"/>
-      <c r="E26" s="203"/>
-      <c r="F26" s="204"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="172"/>
+      <c r="E26" s="174"/>
+      <c r="F26" s="175"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -8526,7 +8539,7 @@
       <c r="T26" s="1"/>
     </row>
     <row r="27" spans="1:22" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="199" t="s">
+      <c r="A27" s="170" t="s">
         <v>373</v>
       </c>
       <c r="B27" s="153">
@@ -8558,7 +8571,7 @@
       <c r="T27" s="1"/>
     </row>
     <row r="28" spans="1:22" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="199" t="s">
+      <c r="A28" s="170" t="s">
         <v>374</v>
       </c>
       <c r="B28" s="153">
@@ -8593,11 +8606,11 @@
       <c r="A29" s="41" t="s">
         <v>370</v>
       </c>
-      <c r="B29" s="201"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="201"/>
-      <c r="E29" s="203"/>
-      <c r="F29" s="204"/>
+      <c r="B29" s="172"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="172"/>
+      <c r="E29" s="174"/>
+      <c r="F29" s="175"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -8614,7 +8627,7 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="1:22" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="200" t="s">
+      <c r="A30" s="171" t="s">
         <v>375</v>
       </c>
       <c r="B30" s="153">
@@ -8646,7 +8659,7 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="1:22" s="33" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="171" t="s">
         <v>376</v>
       </c>
       <c r="B31" s="153">
@@ -8681,11 +8694,11 @@
       <c r="A32" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="205"/>
-      <c r="C32" s="206"/>
-      <c r="D32" s="207"/>
-      <c r="E32" s="208"/>
-      <c r="F32" s="209"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="177"/>
+      <c r="D32" s="178"/>
+      <c r="E32" s="179"/>
+      <c r="F32" s="180"/>
       <c r="G32" s="49"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -9149,12 +9162,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="191" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
       <c r="E1" s="35">
         <f>SUM(E17)</f>
         <v>0</v>
@@ -9232,11 +9245,11 @@
         <v>47</v>
       </c>
       <c r="E6" s="57"/>
-      <c r="F6" s="179" t="s">
+      <c r="F6" s="192" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="179"/>
-      <c r="H6" s="179"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -9391,12 +9404,12 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="180" t="s">
+      <c r="A17" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="180"/>
-      <c r="C17" s="180"/>
-      <c r="D17" s="180"/>
+      <c r="B17" s="193"/>
+      <c r="C17" s="193"/>
+      <c r="D17" s="193"/>
       <c r="E17" s="59">
         <f>SUM(D:D)</f>
         <v>0</v>
@@ -9479,12 +9492,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="194" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
+      <c r="B1" s="194"/>
+      <c r="C1" s="194"/>
+      <c r="D1" s="194"/>
       <c r="E1" s="35">
         <f>SUM(D14)</f>
         <v>0</v>
@@ -9531,18 +9544,18 @@
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="186" t="s">
+      <c r="B3" s="195" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="187" t="s">
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="196" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="187"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="196"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -9581,18 +9594,18 @@
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="197" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="183"/>
-      <c r="D5" s="182">
+      <c r="C5" s="197"/>
+      <c r="D5" s="198">
         <v>0</v>
       </c>
-      <c r="E5" s="182"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
+      <c r="E5" s="198"/>
+      <c r="F5" s="199"/>
+      <c r="G5" s="199"/>
+      <c r="H5" s="199"/>
+      <c r="I5" s="199"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -9608,14 +9621,14 @@
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="183" t="s">
+      <c r="B6" s="197" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="183"/>
-      <c r="D6" s="182">
+      <c r="C6" s="197"/>
+      <c r="D6" s="198">
         <v>0</v>
       </c>
-      <c r="E6" s="182"/>
+      <c r="E6" s="198"/>
       <c r="F6" s="152"/>
       <c r="G6" s="164"/>
       <c r="H6" s="164"/>
@@ -9639,10 +9652,10 @@
         <v>62</v>
       </c>
       <c r="C7" s="68"/>
-      <c r="D7" s="182">
+      <c r="D7" s="198">
         <v>0</v>
       </c>
-      <c r="E7" s="182"/>
+      <c r="E7" s="198"/>
       <c r="F7" s="152"/>
       <c r="G7" s="164"/>
       <c r="H7" s="164"/>
@@ -9666,10 +9679,10 @@
         <v>63</v>
       </c>
       <c r="C8" s="68"/>
-      <c r="D8" s="182">
+      <c r="D8" s="198">
         <v>0</v>
       </c>
-      <c r="E8" s="182"/>
+      <c r="E8" s="198"/>
       <c r="F8" s="152"/>
       <c r="G8" s="164"/>
       <c r="H8" s="164"/>
@@ -9693,10 +9706,10 @@
         <v>64</v>
       </c>
       <c r="C9" s="68"/>
-      <c r="D9" s="182">
+      <c r="D9" s="198">
         <v>0</v>
       </c>
-      <c r="E9" s="182"/>
+      <c r="E9" s="198"/>
       <c r="F9" s="152"/>
       <c r="G9" s="164"/>
       <c r="H9" s="164"/>
@@ -9720,10 +9733,10 @@
         <v>65</v>
       </c>
       <c r="C10" s="68"/>
-      <c r="D10" s="182">
+      <c r="D10" s="198">
         <v>0</v>
       </c>
-      <c r="E10" s="182"/>
+      <c r="E10" s="198"/>
       <c r="F10" s="152"/>
       <c r="G10" s="164"/>
       <c r="H10" s="164"/>
@@ -9743,18 +9756,18 @@
     </row>
     <row r="11" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="183" t="s">
+      <c r="B11" s="197" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="183"/>
-      <c r="D11" s="182">
+      <c r="C11" s="197"/>
+      <c r="D11" s="198">
         <v>0</v>
       </c>
-      <c r="E11" s="182"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="184"/>
-      <c r="H11" s="184"/>
-      <c r="I11" s="184"/>
+      <c r="E11" s="198"/>
+      <c r="F11" s="199"/>
+      <c r="G11" s="199"/>
+      <c r="H11" s="199"/>
+      <c r="I11" s="199"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -9770,18 +9783,18 @@
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="197" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="183"/>
-      <c r="D12" s="182">
+      <c r="C12" s="197"/>
+      <c r="D12" s="198">
         <v>0</v>
       </c>
-      <c r="E12" s="182"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
+      <c r="E12" s="198"/>
+      <c r="F12" s="199"/>
+      <c r="G12" s="199"/>
+      <c r="H12" s="199"/>
+      <c r="I12" s="199"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -9869,13 +9882,13 @@
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="181" t="s">
+      <c r="B16" s="200" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="181"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="181"/>
+      <c r="C16" s="200"/>
+      <c r="D16" s="200"/>
+      <c r="E16" s="200"/>
+      <c r="F16" s="200"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -10766,17 +10779,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B11:C11"/>
@@ -10785,6 +10787,17 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:I12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.37013888888888902" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -10894,16 +10907,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="201" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="196"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="82"/>
@@ -11222,10 +11235,10 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="197" t="s">
+      <c r="A27" s="202" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="197"/>
+      <c r="B27" s="202"/>
       <c r="C27" s="91" t="s">
         <v>131</v>
       </c>
@@ -11235,30 +11248,30 @@
       <c r="E27" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="F27" s="192" t="s">
+      <c r="F27" s="203" t="s">
         <v>134</v>
       </c>
-      <c r="G27" s="192"/>
-      <c r="H27" s="192" t="s">
+      <c r="G27" s="203"/>
+      <c r="H27" s="203" t="s">
         <v>135</v>
       </c>
-      <c r="I27" s="192"/>
-      <c r="J27" s="192" t="s">
+      <c r="I27" s="203"/>
+      <c r="J27" s="203" t="s">
         <v>136</v>
       </c>
-      <c r="K27" s="192"/>
-      <c r="L27" s="192" t="s">
+      <c r="K27" s="203"/>
+      <c r="L27" s="203" t="s">
         <v>137</v>
       </c>
-      <c r="M27" s="192"/>
-      <c r="N27" s="193" t="s">
+      <c r="M27" s="203"/>
+      <c r="N27" s="204" t="s">
         <v>138</v>
       </c>
-      <c r="O27" s="193"/>
-      <c r="Q27" s="194" t="s">
+      <c r="O27" s="204"/>
+      <c r="Q27" s="205" t="s">
         <v>139</v>
       </c>
-      <c r="R27" s="194"/>
+      <c r="R27" s="205"/>
     </row>
     <row r="28" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="93"/>
@@ -11409,10 +11422,10 @@
       <c r="M31" s="103"/>
       <c r="N31" s="93"/>
       <c r="O31" s="93"/>
-      <c r="Q31" s="190" t="s">
+      <c r="Q31" s="206" t="s">
         <v>166</v>
       </c>
-      <c r="R31" s="190"/>
+      <c r="R31" s="206"/>
     </row>
     <row r="32" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="93"/>
@@ -11452,10 +11465,10 @@
       </c>
       <c r="N32" s="93"/>
       <c r="O32" s="93"/>
-      <c r="Q32" s="195" t="s">
+      <c r="Q32" s="207" t="s">
         <v>176</v>
       </c>
-      <c r="R32" s="195"/>
+      <c r="R32" s="207"/>
     </row>
     <row r="33" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="93"/>
@@ -11746,10 +11759,10 @@
       </c>
       <c r="N40" s="93"/>
       <c r="O40" s="93"/>
-      <c r="Q40" s="188" t="s">
+      <c r="Q40" s="208" t="s">
         <v>223</v>
       </c>
-      <c r="R40" s="188"/>
+      <c r="R40" s="208"/>
     </row>
     <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="93"/>
@@ -11789,10 +11802,10 @@
       </c>
       <c r="N41" s="93"/>
       <c r="O41" s="93"/>
-      <c r="Q41" s="189" t="s">
+      <c r="Q41" s="209" t="s">
         <v>231</v>
       </c>
-      <c r="R41" s="189"/>
+      <c r="R41" s="209"/>
     </row>
     <row r="42" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="C42" s="94" t="s">
@@ -12027,10 +12040,10 @@
       <c r="K49" s="93"/>
       <c r="L49" s="93"/>
       <c r="M49" s="93"/>
-      <c r="Q49" s="190" t="s">
+      <c r="Q49" s="206" t="s">
         <v>268</v>
       </c>
-      <c r="R49" s="190"/>
+      <c r="R49" s="206"/>
     </row>
     <row r="50" spans="3:18" ht="15" x14ac:dyDescent="0.25">
       <c r="C50" s="94" t="s">
@@ -12225,10 +12238,10 @@
       <c r="K57" s="93"/>
       <c r="L57" s="93"/>
       <c r="M57" s="93"/>
-      <c r="Q57" s="188" t="s">
+      <c r="Q57" s="208" t="s">
         <v>285</v>
       </c>
-      <c r="R57" s="188"/>
+      <c r="R57" s="208"/>
     </row>
     <row r="58" spans="3:18" ht="15" x14ac:dyDescent="0.25">
       <c r="C58" s="94" t="s">
@@ -12319,11 +12332,11 @@
       <c r="E63" s="127"/>
     </row>
     <row r="64" spans="3:18" ht="44.25" x14ac:dyDescent="0.55000000000000004">
-      <c r="C64" s="191" t="s">
+      <c r="C64" s="210" t="s">
         <v>299</v>
       </c>
-      <c r="D64" s="191"/>
-      <c r="E64" s="191"/>
+      <c r="D64" s="210"/>
+      <c r="E64" s="210"/>
     </row>
     <row r="65" spans="3:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="C65" s="130" t="s">
@@ -12708,21 +12721,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q57:R57"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="Q57:R57"/>
-    <mergeCell ref="C64:E64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -12747,17 +12760,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="198" t="s">
+      <c r="A2" s="211" t="s">
         <v>364</v>
       </c>
-      <c r="B2" s="198"/>
+      <c r="B2" s="211"/>
       <c r="C2" s="149"/>
       <c r="D2" s="149"/>
       <c r="E2" s="149"/>
     </row>
     <row r="3" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="198"/>
-      <c r="B3" s="198"/>
+      <c r="A3" s="211"/>
+      <c r="B3" s="211"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="150" t="s">

</xml_diff>